<commit_message>
calendar and map completed
</commit_message>
<xml_diff>
--- a/shiny_app/data/database.xlsx
+++ b/shiny_app/data/database.xlsx
@@ -1,529 +1,516 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.losi\_personal\Coding\wash_dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paolo.losi\_personal\Coding\wash_sal_dashboard\shiny_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5197C4BE-4F0D-4F44-94F7-E1D330510051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AC8C3D-8F8E-4631-9A26-2AF6D6EDF435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-113" yWindow="-13636" windowWidth="24267" windowHeight="13022" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-113" yWindow="-113" windowWidth="24267" windowHeight="13023" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="advisors" sheetId="1" r:id="rId1"/>
-    <sheet name="wash_list" sheetId="3" r:id="rId2"/>
-    <sheet name="countries" sheetId="2" r:id="rId3"/>
+    <sheet name="wash_list" sheetId="2" r:id="rId2"/>
+    <sheet name="countries" sheetId="3" r:id="rId3"/>
     <sheet name="calendar" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="types" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">countries!$A$1:$B$1</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="159">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>short_name</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>Franck Flachenberg</t>
+  </si>
+  <si>
+    <t>Franck</t>
+  </si>
+  <si>
+    <t>Senior WASH Advisor</t>
+  </si>
+  <si>
+    <t>franck.flachenberg@concern.net</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>Ciaran Mac Mathuma</t>
+  </si>
+  <si>
+    <t>Ciaran</t>
+  </si>
+  <si>
+    <t>Construction Advisor</t>
+  </si>
+  <si>
+    <t>ciaran.macmathuna@concern.net</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>Paolo Losi</t>
+  </si>
+  <si>
+    <t>Paolo</t>
+  </si>
+  <si>
+    <t>WASH Advisor</t>
+  </si>
+  <si>
+    <t>paolo.losi@concern.net</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>Katherine Hardgrave</t>
+  </si>
+  <si>
+    <t>Katherine</t>
+  </si>
+  <si>
+    <t>WASH and Engineering Officer</t>
+  </si>
+  <si>
+    <t>katherine.hardgrave@concern.net</t>
+  </si>
+  <si>
+    <t>sn</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Noor Rahman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afghanistan </t>
+  </si>
+  <si>
+    <t>noor.rhaman@concern.net</t>
+  </si>
+  <si>
+    <t>Koushik Ahamed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangladesh </t>
+  </si>
+  <si>
+    <t>koushik.ahamed@concern.net</t>
+  </si>
+  <si>
+    <t>Ouoba Enos Féhouani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burkina Faso </t>
+  </si>
+  <si>
+    <t>enos.ouoba@concern.net</t>
+  </si>
+  <si>
+    <t>Outayves Eric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central African Republic </t>
+  </si>
+  <si>
+    <t>outayves.eric@concern.net</t>
+  </si>
+  <si>
+    <t>Mahamat Nguini Njoya Moctar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chad </t>
+  </si>
+  <si>
+    <t>mahamat.moctar@concern.net</t>
+  </si>
+  <si>
+    <t>Mougabé Koslengar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congo, Democratic Republic of the </t>
+  </si>
+  <si>
+    <t>mougabe.koslengar@concern.net</t>
+  </si>
+  <si>
+    <t>Tadele Bizuneh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethiopia </t>
+  </si>
+  <si>
+    <t>tadele.bizuneh@concern.net</t>
+  </si>
+  <si>
+    <t>Evans Nyagwaya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kenya </t>
+  </si>
+  <si>
+    <t>evans.nyagwaya@concern.net</t>
+  </si>
+  <si>
+    <t>Sherzada Khan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lebanon </t>
+  </si>
+  <si>
+    <t>sherzada.khan@concern.net</t>
+  </si>
+  <si>
+    <t>Timothy Owhochukwu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liberia </t>
+  </si>
+  <si>
+    <t>timothy.owhochukwu@concern.net</t>
+  </si>
+  <si>
+    <t>Yacine Issoufou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Niger </t>
+  </si>
+  <si>
+    <t>yacine.issoufou@concern.net</t>
+  </si>
+  <si>
+    <t>Yasir Zahir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pakistan </t>
+  </si>
+  <si>
+    <t>yasir.zahir@concern.net</t>
+  </si>
+  <si>
+    <t>Yvan Trapet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rwanda </t>
+  </si>
+  <si>
+    <t>yvan.trapet@concern.net</t>
+  </si>
+  <si>
+    <t>Jusufu Conteh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sierra Leone </t>
+  </si>
+  <si>
+    <t>jusufu.conteh@concern.net</t>
+  </si>
+  <si>
+    <t>Laban Onong’no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somalia </t>
+  </si>
+  <si>
+    <t>laban.onongno@concern.net</t>
+  </si>
+  <si>
+    <t>Khurshid Wisal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Sudan </t>
+  </si>
+  <si>
+    <t>khurshid.wisal@concern.net</t>
+  </si>
+  <si>
+    <t>Subodh Vijapure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sudan </t>
+  </si>
+  <si>
+    <t>subodh.vijapure@concern.net</t>
+  </si>
+  <si>
+    <t>Alex Menendez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Syria </t>
+  </si>
+  <si>
+    <t>alex.menendez@concern.net</t>
+  </si>
+  <si>
+    <t>Abdul Ghaffar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yemen </t>
+  </si>
+  <si>
+    <t>abdul.ghaffar@concern.net</t>
+  </si>
+  <si>
+    <t>Samuel Lamboi</t>
+  </si>
+  <si>
+    <t>samuel.lamboi@concern.net</t>
+  </si>
+  <si>
+    <t>Ali Sayed</t>
+  </si>
+  <si>
+    <t>ali.sayed@concern.net</t>
+  </si>
+  <si>
+    <t>Samson Juhar</t>
+  </si>
+  <si>
+    <t>samson.juhar@concern.net</t>
+  </si>
+  <si>
+    <t>CIA Name</t>
+  </si>
+  <si>
+    <t>ISO 3166 alpha3</t>
+  </si>
+  <si>
+    <t>Continent</t>
+  </si>
+  <si>
+    <t>ta_focal</t>
+  </si>
+  <si>
+    <t>ta_support</t>
+  </si>
+  <si>
+    <t>AFG</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>BGD</t>
+  </si>
+  <si>
+    <t>BFA</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burundi </t>
+  </si>
+  <si>
+    <t>BDI</t>
+  </si>
+  <si>
+    <t>CAF</t>
+  </si>
+  <si>
+    <t>TCD</t>
+  </si>
+  <si>
+    <t>COD</t>
+  </si>
+  <si>
+    <t>ETH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Haiti </t>
+  </si>
+  <si>
+    <t>HTI</t>
+  </si>
+  <si>
+    <t>Americas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iraq </t>
+  </si>
+  <si>
+    <t>IRQ</t>
+  </si>
+  <si>
+    <t>KEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korea, North </t>
+  </si>
+  <si>
+    <t>PRK</t>
+  </si>
+  <si>
+    <t>LBN</t>
+  </si>
+  <si>
+    <t>LBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malawi </t>
+  </si>
+  <si>
+    <t>MWI</t>
+  </si>
+  <si>
+    <t>NER</t>
+  </si>
+  <si>
+    <t>PAK</t>
+  </si>
+  <si>
+    <t>RWA</t>
+  </si>
+  <si>
+    <t>SLE</t>
+  </si>
+  <si>
+    <t>SOM</t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>SDN</t>
+  </si>
+  <si>
+    <t>SYR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey </t>
+  </si>
+  <si>
+    <t>TUR</t>
+  </si>
+  <si>
+    <t>YEM</t>
+  </si>
+  <si>
+    <t>advisor</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>Leave Full Day</t>
+  </si>
+  <si>
+    <t>Bank Holiday</t>
+  </si>
+  <si>
+    <t>Conference/Workshop</t>
+  </si>
+  <si>
+    <t>Climate Workshop Kenya</t>
+  </si>
+  <si>
+    <t>Time In Lieu Full Day</t>
+  </si>
+  <si>
+    <t>Climate, Health Workshop Kenya</t>
+  </si>
+  <si>
+    <t>Country Support Visit</t>
+  </si>
+  <si>
+    <t>Syria</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>GWR Drilling Course</t>
+  </si>
+  <si>
+    <t>Time In Lieu Half Day</t>
+  </si>
   <si>
     <t>Bangladesh</t>
   </si>
   <si>
-    <t>Ethiopia</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>FF</t>
-  </si>
-  <si>
-    <t>Franck Flachenberg</t>
-  </si>
-  <si>
-    <t>Senior WASH Advisor</t>
-  </si>
-  <si>
-    <t>short_name</t>
-  </si>
-  <si>
-    <t>Franck</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>franck.flachenberg@concern.net</t>
-  </si>
-  <si>
-    <t>CM</t>
-  </si>
-  <si>
-    <t>Ciaran Mac Mathuma</t>
-  </si>
-  <si>
-    <t>Ciaran</t>
-  </si>
-  <si>
-    <t>Construction Advisor</t>
-  </si>
-  <si>
-    <t>ciaran.macmathuna@concern.net</t>
-  </si>
-  <si>
-    <t>PL</t>
-  </si>
-  <si>
-    <t>Paolo Losi</t>
-  </si>
-  <si>
-    <t>Paolo</t>
-  </si>
-  <si>
-    <t>WASH Advisor</t>
-  </si>
-  <si>
-    <t>paolo.losi@concern.net</t>
-  </si>
-  <si>
-    <t>KH</t>
-  </si>
-  <si>
-    <t>Katherine Hardgrave</t>
-  </si>
-  <si>
-    <t>Katherine</t>
-  </si>
-  <si>
-    <t>WASH and Engineering Officer</t>
-  </si>
-  <si>
-    <t>katherine.hardgrave@concern.net</t>
-  </si>
-  <si>
-    <t>CIA Name</t>
-  </si>
-  <si>
-    <t>ISO 3166 alpha3</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Sudan </t>
-  </si>
-  <si>
-    <t>SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afghanistan </t>
-  </si>
-  <si>
-    <t>AFG</t>
+    <t>type_code</t>
+  </si>
+  <si>
+    <t>CS</t>
   </si>
   <si>
     <t>BH</t>
   </si>
   <si>
-    <t xml:space="preserve">Bangladesh </t>
-  </si>
-  <si>
-    <t>BGD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burkina Faso </t>
-  </si>
-  <si>
-    <t>BFA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burundi </t>
-  </si>
-  <si>
-    <t>BDI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central African Republic </t>
-  </si>
-  <si>
-    <t>CAF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chad </t>
-  </si>
-  <si>
-    <t>TCD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Congo, Democratic Republic of the </t>
-  </si>
-  <si>
-    <t>COD</t>
+    <t>LFD</t>
+  </si>
+  <si>
+    <t>Leave Half Day</t>
+  </si>
+  <si>
+    <t>LHD</t>
+  </si>
+  <si>
+    <t>LTD</t>
+  </si>
+  <si>
+    <t>LTH</t>
   </si>
   <si>
     <t>CW</t>
   </si>
   <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ethiopia </t>
-  </si>
-  <si>
-    <t>ETH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Haiti </t>
-  </si>
-  <si>
-    <t>HTI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iraq </t>
-  </si>
-  <si>
-    <t>IRQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kenya </t>
-  </si>
-  <si>
-    <t>KEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Korea, North </t>
-  </si>
-  <si>
-    <t>PRK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lebanon </t>
-  </si>
-  <si>
-    <t>LBN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liberia </t>
-  </si>
-  <si>
-    <t>LBR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malawi </t>
-  </si>
-  <si>
-    <t>MWI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Niger </t>
-  </si>
-  <si>
-    <t>NER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pakistan </t>
-  </si>
-  <si>
-    <t>PAK</t>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>Personal Commitment (no travel)</t>
   </si>
   <si>
     <t>PC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rwanda </t>
-  </si>
-  <si>
-    <t>RWA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sierra Leone </t>
-  </si>
-  <si>
-    <t>SLE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Somalia </t>
-  </si>
-  <si>
-    <t>SOM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sudan </t>
-  </si>
-  <si>
-    <t>SDN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Syria </t>
-  </si>
-  <si>
-    <t>SYR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turkey </t>
-  </si>
-  <si>
-    <t>TR</t>
-  </si>
-  <si>
-    <t>TUR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yemen </t>
-  </si>
-  <si>
-    <t>YEM</t>
-  </si>
-  <si>
-    <t>ta_focal</t>
-  </si>
-  <si>
-    <t>ta_support</t>
-  </si>
-  <si>
-    <t>Noor Rahman</t>
-  </si>
-  <si>
-    <t>Koushik Ahamed</t>
-  </si>
-  <si>
-    <t>Ouoba Enos Féhouani</t>
-  </si>
-  <si>
-    <t>Outayves Eric</t>
-  </si>
-  <si>
-    <t>Mahamat Nguini Njoya Moctar</t>
-  </si>
-  <si>
-    <t>Mougabé Koslengar</t>
-  </si>
-  <si>
-    <t>Tadele Bizuneh</t>
-  </si>
-  <si>
-    <t>Evans Nyagwaya</t>
-  </si>
-  <si>
-    <t>Sherzada Khan</t>
-  </si>
-  <si>
-    <t>Timothy Owhochukwu</t>
-  </si>
-  <si>
-    <t>Yacine Issoufou</t>
-  </si>
-  <si>
-    <t>Yasir Zahir</t>
-  </si>
-  <si>
-    <t>Yvan Trapet</t>
-  </si>
-  <si>
-    <t>Jusufu Conteh</t>
-  </si>
-  <si>
-    <t>Laban Onong’no</t>
-  </si>
-  <si>
-    <t>Khurshid Wisal</t>
-  </si>
-  <si>
-    <t>Alex Menendez</t>
-  </si>
-  <si>
-    <t>Abdul Ghaffar</t>
-  </si>
-  <si>
-    <t>Subodh Vijapure</t>
-  </si>
-  <si>
-    <t>noor.rhaman@concern.net</t>
-  </si>
-  <si>
-    <t>koushik.ahamed@concern.net</t>
-  </si>
-  <si>
-    <t>enos.ouoba@concern.net</t>
-  </si>
-  <si>
-    <t>outayves.eric@concern.net</t>
-  </si>
-  <si>
-    <t>mahamat.moctar@concern.net</t>
-  </si>
-  <si>
-    <t>mougabe.koslengar@concern.net</t>
-  </si>
-  <si>
-    <t>tadele.bizuneh@concern.net</t>
-  </si>
-  <si>
-    <t>evans.nyagwaya@concern.net</t>
-  </si>
-  <si>
-    <t>sherzada.khan@concern.net</t>
-  </si>
-  <si>
-    <t>timothy.owhochukwu@concern.net</t>
-  </si>
-  <si>
-    <t>yacine.issoufou@concern.net</t>
-  </si>
-  <si>
-    <t>sn</t>
-  </si>
-  <si>
-    <t>yasir.zahir@concern.net</t>
-  </si>
-  <si>
-    <t>yvan.trapet@concern.net</t>
-  </si>
-  <si>
-    <t>jusufu.conteh@concern.net</t>
-  </si>
-  <si>
-    <t>khurshid.wisal@concern.net</t>
-  </si>
-  <si>
-    <t>subodh.vijapure@concern.net</t>
-  </si>
-  <si>
-    <t>alex.menendez@concern.net</t>
-  </si>
-  <si>
-    <t>abdul.ghaffar@concern.net</t>
-  </si>
-  <si>
-    <t>laban.onongno@concern.net</t>
-  </si>
-  <si>
-    <t>Samuel Lamboi</t>
-  </si>
-  <si>
-    <t>samuel.lamboi@concern.net</t>
-  </si>
-  <si>
-    <t>Ali Sayed</t>
-  </si>
-  <si>
-    <t>ali.sayed@concern.net</t>
-  </si>
-  <si>
-    <t>Samson Juhar</t>
-  </si>
-  <si>
-    <t>samson.juhar@concern.net</t>
-  </si>
-  <si>
-    <t>advisor</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>end_date</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>Country Support Visit</t>
-  </si>
-  <si>
-    <t>Conference/Workshop</t>
-  </si>
-  <si>
-    <t>Personal Commitment (no travel)</t>
-  </si>
-  <si>
-    <t>Bank Holiday</t>
-  </si>
-  <si>
-    <t>remarks</t>
-  </si>
-  <si>
-    <t>Climate Workshop Kenya</t>
-  </si>
-  <si>
-    <t>Climate, Health Workshop Kenya</t>
-  </si>
-  <si>
-    <t>Syria</t>
-  </si>
-  <si>
-    <t>Training</t>
-  </si>
-  <si>
-    <t>GWR Drilling Course</t>
-  </si>
-  <si>
-    <t>Leave Full Day</t>
-  </si>
-  <si>
-    <t>Leave Half Day</t>
-  </si>
-  <si>
-    <t>Time In Lieu Full Day</t>
-  </si>
-  <si>
-    <t>Time In Lieu Half Day</t>
-  </si>
-  <si>
-    <t>LTH</t>
-  </si>
-  <si>
-    <t>LFD</t>
-  </si>
-  <si>
-    <t>LHD</t>
-  </si>
-  <si>
-    <t>LTD</t>
-  </si>
-  <si>
-    <t>Africa</t>
-  </si>
-  <si>
-    <t>Continent</t>
-  </si>
-  <si>
-    <t>Asia</t>
-  </si>
-  <si>
-    <t>Americas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -539,6 +526,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -548,7 +540,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -556,28 +548,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -588,20 +591,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0D8F7AEA-04A1-44E1-8555-9D141BCEB7B2}" name="Table1" displayName="Table1" ref="A1:E24" totalsRowShown="0">
-  <autoFilter ref="A1:E24" xr:uid="{0D8F7AEA-04A1-44E1-8555-9D141BCEB7B2}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4500F812-437A-4DEC-B6B1-22FB795A2E47}" name="advisor"/>
-    <tableColumn id="2" xr3:uid="{5176497F-2F40-4917-AAF5-BFBC7105A582}" name="start_date" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{44EC0D7F-8188-4B30-96A1-83219EC22A09}" name="end_date" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{340B95B8-1107-4DF5-BB4A-004285A08637}" name="type"/>
-    <tableColumn id="5" xr3:uid="{9C5750B8-2984-4192-9D1B-27519DB72833}" name="remarks"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -884,19 +873,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -907,79 +896,79 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{04718FEA-43AD-4593-A875-EC53392927A5}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{12966451-6C63-46E7-AA8F-74E990848C59}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{26723F6F-34E8-4ED3-93C6-8660257CB8D5}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{C0C821B1-177E-4239-AEE3-0CA70E720F98}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF181D4C-E66F-4019-9E0C-A503F124D30C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -996,19 +985,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1016,13 +1005,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>106</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1030,13 +1019,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1044,13 +1033,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1058,13 +1047,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1072,13 +1061,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>110</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1086,13 +1075,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1100,13 +1089,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>112</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1114,13 +1103,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1128,13 +1117,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1142,13 +1131,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>115</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1156,13 +1145,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1170,13 +1159,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>118</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1184,13 +1173,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>119</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1198,13 +1187,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1212,13 +1201,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1226,13 +1215,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>121</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1240,13 +1229,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
         <v>76</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1254,13 +1243,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1268,13 +1257,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1282,13 +1271,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>84</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>127</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1296,13 +1285,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1310,62 +1299,50 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>131</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{9A741FC0-54A2-4811-B1A5-134FB3E4A1AC}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{52BFCC4D-522D-4FB6-B423-D6CF74E909A0}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{F80013FE-2812-4DA7-B15F-1D67A6E22CD3}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{4935D365-89ED-4DFE-96D2-BBEA48EEB38C}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{00557844-75C1-4AE8-ACBF-DD0265A13942}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{6161CB53-1D75-4A1B-A273-C53E4FC117B1}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{05AD02AE-615A-45E8-8E40-110CE0BDE84B}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{75055243-5434-471E-8551-A9462C50A9FE}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{9D259CEF-C1CE-4669-A9BC-0CA355DDF5EC}"/>
-    <hyperlink ref="E11" r:id="rId10" xr:uid="{CD3EAC01-9954-4B27-9729-08FD711C6DC2}"/>
-    <hyperlink ref="E12" r:id="rId11" xr:uid="{9C682B23-1B45-4C79-8C49-57A0EAA1D187}"/>
-    <hyperlink ref="E13" r:id="rId12" xr:uid="{F5F48C8A-4FC1-4321-8AC6-0D790F39A741}"/>
-    <hyperlink ref="E14" r:id="rId13" xr:uid="{61231DD2-A847-40E1-926D-132840948A76}"/>
-    <hyperlink ref="E15" r:id="rId14" xr:uid="{EB690CFF-8203-4326-9BA5-BDCE9FE754E1}"/>
-    <hyperlink ref="E16" r:id="rId15" xr:uid="{4F78A0A3-1EF1-4AE5-8574-CF53CA3C5D81}"/>
-    <hyperlink ref="E17" r:id="rId16" xr:uid="{CE3B091F-8363-4A10-A33F-CC978227F05C}"/>
-    <hyperlink ref="E18" r:id="rId17" xr:uid="{F0C7F182-18E8-4F51-917E-015E0A9D11B0}"/>
-    <hyperlink ref="E19" r:id="rId18" xr:uid="{F6457FD5-0C56-4645-B6FC-7F134E178B53}"/>
-    <hyperlink ref="E20" r:id="rId19" xr:uid="{43B2FA63-C5DE-471F-9259-2DAB99F5A4D1}"/>
-    <hyperlink ref="E21" r:id="rId20" xr:uid="{E27D7BCB-2F80-4A17-B266-3CAF552D8E6C}"/>
-    <hyperlink ref="E22" r:id="rId21" xr:uid="{F2220BC4-CA3C-4A48-8CF2-2223FB512D94}"/>
-    <hyperlink ref="E23" r:id="rId22" xr:uid="{4ED32163-3921-459E-94F1-24E248E3F3E3}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0DC26CFD-1098-470A-BC72-BE8C1917E995}">
-          <x14:formula1>
-            <xm:f>countries!$A$2:$A$26</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C23</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F108BA34-3429-4595-9E61-1EDF2937C977}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1379,325 +1356,325 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="C1" t="s">
-        <v>155</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>101</v>
       </c>
       <c r="C5" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>114</v>
       </c>
       <c r="C14" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B17" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>120</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="C20" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>75</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1705,114 +1682,101 @@
         <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B24" t="s">
-        <v>79</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>80</v>
+        <v>126</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="C25" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" t="s">
-        <v>84</v>
+        <v>128</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4F0734BB-EE8E-4DAD-9921-508F9D6F0FE9}">
-          <x14:formula1>
-            <xm:f>advisors!$C$2:$C$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:E26</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FF3AFC-EF06-4C1B-9CC9-98A5EA8BF0FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="C1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2">
         <v>45644</v>
@@ -1821,12 +1785,12 @@
         <v>45650</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3" s="2">
         <v>45651</v>
@@ -1835,12 +1799,12 @@
         <v>45653</v>
       </c>
       <c r="D3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <v>45656</v>
@@ -1849,12 +1813,12 @@
         <v>45657</v>
       </c>
       <c r="D4" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="2">
         <v>45658</v>
@@ -1863,12 +1827,12 @@
         <v>45658</v>
       </c>
       <c r="D5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2">
         <v>45597</v>
@@ -1877,15 +1841,15 @@
         <v>45597</v>
       </c>
       <c r="D6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" t="s">
         <v>137</v>
-      </c>
-      <c r="E6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>45603</v>
@@ -1894,12 +1858,12 @@
         <v>45604</v>
       </c>
       <c r="D7" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
         <v>45597</v>
@@ -1908,15 +1872,15 @@
         <v>45604</v>
       </c>
       <c r="D8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>45618</v>
@@ -1925,15 +1889,15 @@
         <v>45627</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="2">
         <v>45651</v>
@@ -1942,12 +1906,12 @@
         <v>45653</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="2">
         <v>45656</v>
@@ -1956,12 +1920,12 @@
         <v>45657</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B12" s="2">
         <v>45658</v>
@@ -1970,12 +1934,12 @@
         <v>45658</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2">
         <v>45597</v>
@@ -1984,15 +1948,15 @@
         <v>45597</v>
       </c>
       <c r="D13" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>45602</v>
@@ -2001,15 +1965,15 @@
         <v>45604</v>
       </c>
       <c r="D14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" t="s">
         <v>144</v>
-      </c>
-      <c r="E14" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2">
         <v>45609</v>
@@ -2018,12 +1982,12 @@
         <v>45611</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>45624</v>
@@ -2032,12 +1996,12 @@
         <v>45624</v>
       </c>
       <c r="D16" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="2">
         <v>45651</v>
@@ -2046,12 +2010,12 @@
         <v>45653</v>
       </c>
       <c r="D17" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2">
         <v>45656</v>
@@ -2060,12 +2024,12 @@
         <v>45657</v>
       </c>
       <c r="D18" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2">
         <v>45658</v>
@@ -2074,12 +2038,12 @@
         <v>45658</v>
       </c>
       <c r="D19" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B20" s="2">
         <v>45617</v>
@@ -2088,15 +2052,15 @@
         <v>45631</v>
       </c>
       <c r="D20" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E20" t="s">
-        <v>0</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" s="2">
         <v>45638</v>
@@ -2105,12 +2069,12 @@
         <v>45638</v>
       </c>
       <c r="D21" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22" s="2">
         <v>45651</v>
@@ -2119,12 +2083,12 @@
         <v>45653</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23" s="2">
         <v>45656</v>
@@ -2133,12 +2097,12 @@
         <v>45657</v>
       </c>
       <c r="D23" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24" s="2">
         <v>45658</v>
@@ -2147,46 +2111,20 @@
         <v>45658</v>
       </c>
       <c r="D24" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:C24" xr:uid="{2EE9EE4E-8FF4-4458-8785-BFE4FD977EA8}">
-      <formula1>45292</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E64527A-30B3-4698-9854-804F4F00D91B}">
-          <x14:formula1>
-            <xm:f>advisors!$C$2:$C$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A24</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5EBD1DC3-1B79-4B83-88E5-6075EBB306CF}">
-          <x14:formula1>
-            <xm:f>Sheet4!$A$2:$A$10</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D24</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE2AFEF-496B-4A19-AF69-4B9F3971F1F5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -2196,36 +2134,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B5" t="s">
         <v>152</v>
@@ -2233,7 +2174,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B6" t="s">
         <v>153</v>
@@ -2241,34 +2182,34 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>